<commit_message>
Fixed Kinetic Energy Matrix Computation via Integration
</commit_message>
<xml_diff>
--- a/Vibrational Energy & Wavefunctions/Efficiency_Data.xlsx
+++ b/Vibrational Energy & Wavefunctions/Efficiency_Data.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\School\Chapman\Research\QM\CatLab_CompChem\Vibrational Energy &amp; Wavefunctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1A015B-FBCD-47C3-B84C-7DA452DC71C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CAECB4-CCE4-4512-99B0-A49A1727CFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{B4084FC0-2347-43AB-9E40-61F26FA15E8C}"/>
+    <workbookView xWindow="210" yWindow="2130" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{B4084FC0-2347-43AB-9E40-61F26FA15E8C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="VE&amp;WF EFF" sheetId="1" r:id="rId1"/>
+    <sheet name="VE&amp;WF TINT" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$L$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VE&amp;WF EFF'!$A$1:$L$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="30">
   <si>
     <t>RE @ Zero</t>
   </si>
@@ -97,10 +97,37 @@
     <t>v=10</t>
   </si>
   <si>
-    <t>H2</t>
-  </si>
-  <si>
     <t>Builds Half V</t>
+  </si>
+  <si>
+    <t>Basis 1</t>
+  </si>
+  <si>
+    <t>Basis 2</t>
+  </si>
+  <si>
+    <t>Integrand Graph</t>
+  </si>
+  <si>
+    <t>dx Value</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Scipy || MPMath</t>
+  </si>
+  <si>
+    <t>Scipy</t>
+  </si>
+  <si>
+    <t>Using *2Pi for HOW</t>
+  </si>
+  <si>
+    <t>Derivative</t>
+  </si>
+  <si>
+    <t>n=1</t>
   </si>
 </sst>
 </file>
@@ -171,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -184,6 +211,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -200,6 +230,254 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1171575" cy="1415403"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9984C61E-0A8A-46AD-ABE5-375394C31436}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="3241" r="57509"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4057650" y="609600"/>
+          <a:ext cx="1171575" cy="1415403"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1666875" cy="1260475"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{313729E1-8483-47E6-841A-0B2B921781F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3943350" y="2162175"/>
+          <a:ext cx="1666875" cy="1260475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1066800" cy="1349664"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE178158-7EDD-46C2-8DDE-C22A97FEB863}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276726" y="3476625"/>
+          <a:ext cx="1066800" cy="1349664"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>27819</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1143000" cy="1391845"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9EF028-4D95-49F7-9E05-37B69A978235}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267201" y="4914144"/>
+          <a:ext cx="1143000" cy="1391845"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1353346</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{853EF4D8-9B5D-4696-81A9-563730A53243}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5562601" y="6438900"/>
+          <a:ext cx="952499" cy="1229521"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1631767</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F397C9D-1D83-4CCD-9A7D-51F04B6E978F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5534025" y="7781924"/>
+          <a:ext cx="1250767" cy="1400176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,12 +777,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126B9875-771B-47F6-B347-9268AE11311E}">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +822,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -1743,186 +2021,6 @@
         <v>9</v>
       </c>
       <c r="H47" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D48" s="4">
-        <v>2</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" s="4">
-        <v>3</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="4">
-        <v>4</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H50" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="4">
-        <v>5</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D52" s="4">
-        <v>6</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C53" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" s="4">
-        <v>7</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H53" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" s="4">
-        <v>8</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H54" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D55" s="4">
-        <v>9</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H55" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C56" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" s="4">
-        <v>10</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H56" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1932,4 +2030,214 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D2F791-7B0E-43B3-B94E-24AEF48D98D2}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="112.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="12.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="19.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Duplicate Classes Issue
</commit_message>
<xml_diff>
--- a/Vibrational Energy & Wavefunctions/Efficiency_Data.xlsx
+++ b/Vibrational Energy & Wavefunctions/Efficiency_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\School\Chapman\Research\QM\CatLab_CompChem\Vibrational Energy &amp; Wavefunctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CAECB4-CCE4-4512-99B0-A49A1727CFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73087FE1-FC4D-433D-A360-F710699134F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="2130" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{B4084FC0-2347-43AB-9E40-61F26FA15E8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4084FC0-2347-43AB-9E40-61F26FA15E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="VE&amp;WF EFF" sheetId="1" r:id="rId1"/>
@@ -779,10 +779,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126B9875-771B-47F6-B347-9268AE11311E}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D2F791-7B0E-43B3-B94E-24AEF48D98D2}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>